<commit_message>
Gestion de projet - parties_prenantes.png - matrice_des_objectifs.png - exemple_rapport.jpeg
</commit_message>
<xml_diff>
--- a/doc/livrable_1/rapport/templates/gantt.xlsx
+++ b/doc/livrable_1/rapport/templates/gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33BA2883-725B-42D6-8BA9-EFE5B9FC5D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{C9655527-7F3E-417B-AA5C-08656AAAE3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1911,8 +1911,8 @@
   <dimension ref="A1:DP36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1959,8 +1959,8 @@
       </c>
       <c r="D3" s="66"/>
       <c r="E3" s="70">
-        <f ca="1">TODAY()-10</f>
-        <v>44843</v>
+        <f ca="1">TODAY()-9</f>
+        <v>44844</v>
       </c>
       <c r="F3" s="70"/>
     </row>
@@ -2105,36 +2105,6 @@
       <c r="CS4" s="68"/>
       <c r="CT4" s="68"/>
       <c r="CU4" s="69"/>
-      <c r="CV4" s="67">
-        <f ca="1">CV5</f>
-        <v>44935</v>
-      </c>
-      <c r="CW4" s="68"/>
-      <c r="CX4" s="68"/>
-      <c r="CY4" s="68"/>
-      <c r="CZ4" s="68"/>
-      <c r="DA4" s="68"/>
-      <c r="DB4" s="69"/>
-      <c r="DC4" s="67">
-        <f ca="1">DC5</f>
-        <v>44942</v>
-      </c>
-      <c r="DD4" s="68"/>
-      <c r="DE4" s="68"/>
-      <c r="DF4" s="68"/>
-      <c r="DG4" s="68"/>
-      <c r="DH4" s="68"/>
-      <c r="DI4" s="69"/>
-      <c r="DJ4" s="67">
-        <f ca="1">DJ5</f>
-        <v>44949</v>
-      </c>
-      <c r="DK4" s="68"/>
-      <c r="DL4" s="68"/>
-      <c r="DM4" s="68"/>
-      <c r="DN4" s="68"/>
-      <c r="DO4" s="68"/>
-      <c r="DP4" s="69"/>
     </row>
     <row r="5" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
@@ -2510,90 +2480,6 @@
         <f t="shared" ref="CU5" ca="1" si="27">CT5+1</f>
         <v>44934</v>
       </c>
-      <c r="CV5" s="11">
-        <f ca="1">CU5+1</f>
-        <v>44935</v>
-      </c>
-      <c r="CW5" s="10">
-        <f ca="1">CV5+1</f>
-        <v>44936</v>
-      </c>
-      <c r="CX5" s="10">
-        <f t="shared" ref="CX5" ca="1" si="28">CW5+1</f>
-        <v>44937</v>
-      </c>
-      <c r="CY5" s="10">
-        <f t="shared" ref="CY5" ca="1" si="29">CX5+1</f>
-        <v>44938</v>
-      </c>
-      <c r="CZ5" s="10">
-        <f t="shared" ref="CZ5" ca="1" si="30">CY5+1</f>
-        <v>44939</v>
-      </c>
-      <c r="DA5" s="10">
-        <f t="shared" ref="DA5" ca="1" si="31">CZ5+1</f>
-        <v>44940</v>
-      </c>
-      <c r="DB5" s="12">
-        <f t="shared" ref="DB5" ca="1" si="32">DA5+1</f>
-        <v>44941</v>
-      </c>
-      <c r="DC5" s="11">
-        <f ca="1">DB5+1</f>
-        <v>44942</v>
-      </c>
-      <c r="DD5" s="10">
-        <f ca="1">DC5+1</f>
-        <v>44943</v>
-      </c>
-      <c r="DE5" s="10">
-        <f t="shared" ref="DE5" ca="1" si="33">DD5+1</f>
-        <v>44944</v>
-      </c>
-      <c r="DF5" s="10">
-        <f t="shared" ref="DF5" ca="1" si="34">DE5+1</f>
-        <v>44945</v>
-      </c>
-      <c r="DG5" s="10">
-        <f t="shared" ref="DG5" ca="1" si="35">DF5+1</f>
-        <v>44946</v>
-      </c>
-      <c r="DH5" s="10">
-        <f t="shared" ref="DH5" ca="1" si="36">DG5+1</f>
-        <v>44947</v>
-      </c>
-      <c r="DI5" s="12">
-        <f t="shared" ref="DI5" ca="1" si="37">DH5+1</f>
-        <v>44948</v>
-      </c>
-      <c r="DJ5" s="11">
-        <f ca="1">DI5+1</f>
-        <v>44949</v>
-      </c>
-      <c r="DK5" s="10">
-        <f ca="1">DJ5+1</f>
-        <v>44950</v>
-      </c>
-      <c r="DL5" s="10">
-        <f t="shared" ref="DL5" ca="1" si="38">DK5+1</f>
-        <v>44951</v>
-      </c>
-      <c r="DM5" s="10">
-        <f t="shared" ref="DM5" ca="1" si="39">DL5+1</f>
-        <v>44952</v>
-      </c>
-      <c r="DN5" s="10">
-        <f t="shared" ref="DN5" ca="1" si="40">DM5+1</f>
-        <v>44953</v>
-      </c>
-      <c r="DO5" s="10">
-        <f t="shared" ref="DO5" ca="1" si="41">DN5+1</f>
-        <v>44954</v>
-      </c>
-      <c r="DP5" s="12">
-        <f t="shared" ref="DP5" ca="1" si="42">DO5+1</f>
-        <v>44955</v>
-      </c>
     </row>
     <row r="6" spans="1:120" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="43" t="s">
@@ -2619,451 +2505,367 @@
         <v>6</v>
       </c>
       <c r="I6" s="13" t="str">
-        <f t="shared" ref="I6" ca="1" si="43">LEFT(TEXT(I5,"ddd"),1)</f>
+        <f t="shared" ref="I6" ca="1" si="28">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="J6" s="13" t="str">
-        <f t="shared" ref="J6:AR6" ca="1" si="44">LEFT(TEXT(J5,"ddd"),1)</f>
+        <f t="shared" ref="J6:AR6" ca="1" si="29">LEFT(TEXT(J5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="K6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="L6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="M6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="N6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="O6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="P6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="Q6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="R6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="S6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="T6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="U6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="V6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="W6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="X6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="Y6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="Z6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AA6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AB6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AC6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AD6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AE6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AF6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AG6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AH6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AI6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AJ6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AK6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AL6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AM6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AN6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AO6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AP6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AQ6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AR6" s="13" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" ca="1" si="29"/>
         <v>d</v>
       </c>
       <c r="AS6" s="13" t="str">
-        <f t="shared" ref="AS6:BL6" ca="1" si="45">LEFT(TEXT(AS5,"ddd"),1)</f>
+        <f t="shared" ref="AS6:BL6" ca="1" si="30">LEFT(TEXT(AS5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="AT6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="AU6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="AV6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="AW6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="AX6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="AY6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="AZ6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BA6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BB6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BC6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BD6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BE6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BF6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BG6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BH6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BI6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BJ6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BK6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BL6" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="30"/>
         <v>d</v>
       </c>
       <c r="BM6" s="13" t="str">
-        <f t="shared" ref="BM6:DP6" ca="1" si="46">LEFT(TEXT(BM5,"ddd"),1)</f>
+        <f t="shared" ref="BM6:DP6" ca="1" si="31">LEFT(TEXT(BM5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="BN6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BO6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BP6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BQ6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BR6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BS6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BT6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BU6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BV6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BW6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BX6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BY6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="BZ6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CA6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CB6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CC6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CD6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CE6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CF6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CG6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CH6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CI6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CJ6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CK6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CL6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CM6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CN6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CO6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CP6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CQ6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CR6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CS6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CT6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
       <c r="CU6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="CV6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="CW6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="CX6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="CY6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="CZ6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DA6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DB6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DC6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DD6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DE6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DF6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DG6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DH6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DI6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DJ6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DK6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DL6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DM6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DN6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DO6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>d</v>
-      </c>
-      <c r="DP6" s="13" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="31"/>
         <v>d</v>
       </c>
     </row>
@@ -3168,27 +2970,6 @@
       <c r="CS7" s="29"/>
       <c r="CT7" s="29"/>
       <c r="CU7" s="29"/>
-      <c r="CV7" s="29"/>
-      <c r="CW7" s="29"/>
-      <c r="CX7" s="29"/>
-      <c r="CY7" s="29"/>
-      <c r="CZ7" s="29"/>
-      <c r="DA7" s="29"/>
-      <c r="DB7" s="29"/>
-      <c r="DC7" s="29"/>
-      <c r="DD7" s="29"/>
-      <c r="DE7" s="29"/>
-      <c r="DF7" s="29"/>
-      <c r="DG7" s="29"/>
-      <c r="DH7" s="29"/>
-      <c r="DI7" s="29"/>
-      <c r="DJ7" s="29"/>
-      <c r="DK7" s="29"/>
-      <c r="DL7" s="29"/>
-      <c r="DM7" s="29"/>
-      <c r="DN7" s="29"/>
-      <c r="DO7" s="29"/>
-      <c r="DP7" s="29"/>
     </row>
     <row r="8" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="43" t="s">
@@ -3203,7 +2984,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="str">
-        <f t="shared" ref="H8:H25" si="47">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H25" si="32">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="29"/>
@@ -3297,27 +3078,27 @@
       <c r="CS8" s="29"/>
       <c r="CT8" s="29"/>
       <c r="CU8" s="29"/>
-      <c r="CV8" s="29"/>
-      <c r="CW8" s="29"/>
-      <c r="CX8" s="29"/>
-      <c r="CY8" s="29"/>
-      <c r="CZ8" s="29"/>
-      <c r="DA8" s="29"/>
-      <c r="DB8" s="29"/>
-      <c r="DC8" s="29"/>
-      <c r="DD8" s="29"/>
-      <c r="DE8" s="29"/>
-      <c r="DF8" s="29"/>
-      <c r="DG8" s="29"/>
-      <c r="DH8" s="29"/>
-      <c r="DI8" s="29"/>
-      <c r="DJ8" s="29"/>
-      <c r="DK8" s="29"/>
-      <c r="DL8" s="29"/>
-      <c r="DM8" s="29"/>
-      <c r="DN8" s="29"/>
-      <c r="DO8" s="29"/>
-      <c r="DP8" s="29"/>
+      <c r="CV8"/>
+      <c r="CW8"/>
+      <c r="CX8"/>
+      <c r="CY8"/>
+      <c r="CZ8"/>
+      <c r="DA8"/>
+      <c r="DB8"/>
+      <c r="DC8"/>
+      <c r="DD8"/>
+      <c r="DE8"/>
+      <c r="DF8"/>
+      <c r="DG8"/>
+      <c r="DH8"/>
+      <c r="DI8"/>
+      <c r="DJ8"/>
+      <c r="DK8"/>
+      <c r="DL8"/>
+      <c r="DM8"/>
+      <c r="DN8"/>
+      <c r="DO8"/>
+      <c r="DP8"/>
     </row>
     <row r="9" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="43" t="s">
@@ -3330,16 +3111,16 @@
       <c r="D9" s="21"/>
       <c r="E9" s="49">
         <f ca="1">Project_Start</f>
-        <v>44843</v>
+        <v>44844</v>
       </c>
       <c r="F9" s="49">
-        <f ca="1">E9+2</f>
+        <f ca="1">E9+1</f>
         <v>44845</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16">
-        <f t="shared" ca="1" si="47"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="32"/>
+        <v>2</v>
       </c>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
@@ -3432,27 +3213,27 @@
       <c r="CS9" s="29"/>
       <c r="CT9" s="29"/>
       <c r="CU9" s="29"/>
-      <c r="CV9" s="29"/>
-      <c r="CW9" s="29"/>
-      <c r="CX9" s="29"/>
-      <c r="CY9" s="29"/>
-      <c r="CZ9" s="29"/>
-      <c r="DA9" s="29"/>
-      <c r="DB9" s="29"/>
-      <c r="DC9" s="29"/>
-      <c r="DD9" s="29"/>
-      <c r="DE9" s="29"/>
-      <c r="DF9" s="29"/>
-      <c r="DG9" s="29"/>
-      <c r="DH9" s="29"/>
-      <c r="DI9" s="29"/>
-      <c r="DJ9" s="29"/>
-      <c r="DK9" s="29"/>
-      <c r="DL9" s="29"/>
-      <c r="DM9" s="29"/>
-      <c r="DN9" s="29"/>
-      <c r="DO9" s="29"/>
-      <c r="DP9" s="29"/>
+      <c r="CV9"/>
+      <c r="CW9"/>
+      <c r="CX9"/>
+      <c r="CY9"/>
+      <c r="CZ9"/>
+      <c r="DA9"/>
+      <c r="DB9"/>
+      <c r="DC9"/>
+      <c r="DD9"/>
+      <c r="DE9"/>
+      <c r="DF9"/>
+      <c r="DG9"/>
+      <c r="DH9"/>
+      <c r="DI9"/>
+      <c r="DJ9"/>
+      <c r="DK9"/>
+      <c r="DL9"/>
+      <c r="DM9"/>
+      <c r="DN9"/>
+      <c r="DO9"/>
+      <c r="DP9"/>
     </row>
     <row r="10" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="43" t="s">
@@ -3473,7 +3254,7 @@
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>3</v>
       </c>
       <c r="I10" s="29"/>
@@ -3567,27 +3348,27 @@
       <c r="CS10" s="29"/>
       <c r="CT10" s="29"/>
       <c r="CU10" s="29"/>
-      <c r="CV10" s="29"/>
-      <c r="CW10" s="29"/>
-      <c r="CX10" s="29"/>
-      <c r="CY10" s="29"/>
-      <c r="CZ10" s="29"/>
-      <c r="DA10" s="29"/>
-      <c r="DB10" s="29"/>
-      <c r="DC10" s="29"/>
-      <c r="DD10" s="29"/>
-      <c r="DE10" s="29"/>
-      <c r="DF10" s="29"/>
-      <c r="DG10" s="29"/>
-      <c r="DH10" s="29"/>
-      <c r="DI10" s="29"/>
-      <c r="DJ10" s="29"/>
-      <c r="DK10" s="29"/>
-      <c r="DL10" s="29"/>
-      <c r="DM10" s="29"/>
-      <c r="DN10" s="29"/>
-      <c r="DO10" s="29"/>
-      <c r="DP10" s="29"/>
+      <c r="CV10"/>
+      <c r="CW10"/>
+      <c r="CX10"/>
+      <c r="CY10"/>
+      <c r="CZ10"/>
+      <c r="DA10"/>
+      <c r="DB10"/>
+      <c r="DC10"/>
+      <c r="DD10"/>
+      <c r="DE10"/>
+      <c r="DF10"/>
+      <c r="DG10"/>
+      <c r="DH10"/>
+      <c r="DI10"/>
+      <c r="DJ10"/>
+      <c r="DK10"/>
+      <c r="DL10"/>
+      <c r="DM10"/>
+      <c r="DN10"/>
+      <c r="DO10"/>
+      <c r="DP10"/>
     </row>
     <row r="11" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="42"/>
@@ -3606,7 +3387,7 @@
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>5</v>
       </c>
       <c r="I11" s="29"/>
@@ -3700,27 +3481,27 @@
       <c r="CS11" s="29"/>
       <c r="CT11" s="29"/>
       <c r="CU11" s="29"/>
-      <c r="CV11" s="29"/>
-      <c r="CW11" s="29"/>
-      <c r="CX11" s="29"/>
-      <c r="CY11" s="29"/>
-      <c r="CZ11" s="29"/>
-      <c r="DA11" s="29"/>
-      <c r="DB11" s="29"/>
-      <c r="DC11" s="29"/>
-      <c r="DD11" s="29"/>
-      <c r="DE11" s="29"/>
-      <c r="DF11" s="29"/>
-      <c r="DG11" s="29"/>
-      <c r="DH11" s="29"/>
-      <c r="DI11" s="29"/>
-      <c r="DJ11" s="29"/>
-      <c r="DK11" s="29"/>
-      <c r="DL11" s="29"/>
-      <c r="DM11" s="29"/>
-      <c r="DN11" s="29"/>
-      <c r="DO11" s="29"/>
-      <c r="DP11" s="29"/>
+      <c r="CV11"/>
+      <c r="CW11"/>
+      <c r="CX11"/>
+      <c r="CY11"/>
+      <c r="CZ11"/>
+      <c r="DA11"/>
+      <c r="DB11"/>
+      <c r="DC11"/>
+      <c r="DD11"/>
+      <c r="DE11"/>
+      <c r="DF11"/>
+      <c r="DG11"/>
+      <c r="DH11"/>
+      <c r="DI11"/>
+      <c r="DJ11"/>
+      <c r="DK11"/>
+      <c r="DL11"/>
+      <c r="DM11"/>
+      <c r="DN11"/>
+      <c r="DO11"/>
+      <c r="DP11"/>
     </row>
     <row r="12" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="42"/>
@@ -3739,7 +3520,7 @@
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>6</v>
       </c>
       <c r="I12" s="29"/>
@@ -3833,27 +3614,27 @@
       <c r="CS12" s="29"/>
       <c r="CT12" s="29"/>
       <c r="CU12" s="29"/>
-      <c r="CV12" s="29"/>
-      <c r="CW12" s="29"/>
-      <c r="CX12" s="29"/>
-      <c r="CY12" s="29"/>
-      <c r="CZ12" s="29"/>
-      <c r="DA12" s="29"/>
-      <c r="DB12" s="29"/>
-      <c r="DC12" s="29"/>
-      <c r="DD12" s="29"/>
-      <c r="DE12" s="29"/>
-      <c r="DF12" s="29"/>
-      <c r="DG12" s="29"/>
-      <c r="DH12" s="29"/>
-      <c r="DI12" s="29"/>
-      <c r="DJ12" s="29"/>
-      <c r="DK12" s="29"/>
-      <c r="DL12" s="29"/>
-      <c r="DM12" s="29"/>
-      <c r="DN12" s="29"/>
-      <c r="DO12" s="29"/>
-      <c r="DP12" s="29"/>
+      <c r="CV12"/>
+      <c r="CW12"/>
+      <c r="CX12"/>
+      <c r="CY12"/>
+      <c r="CZ12"/>
+      <c r="DA12"/>
+      <c r="DB12"/>
+      <c r="DC12"/>
+      <c r="DD12"/>
+      <c r="DE12"/>
+      <c r="DF12"/>
+      <c r="DG12"/>
+      <c r="DH12"/>
+      <c r="DI12"/>
+      <c r="DJ12"/>
+      <c r="DK12"/>
+      <c r="DL12"/>
+      <c r="DM12"/>
+      <c r="DN12"/>
+      <c r="DO12"/>
+      <c r="DP12"/>
     </row>
     <row r="13" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="42"/>
@@ -3872,7 +3653,7 @@
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>1</v>
       </c>
       <c r="I13" s="29"/>
@@ -3966,27 +3747,27 @@
       <c r="CS13" s="29"/>
       <c r="CT13" s="29"/>
       <c r="CU13" s="29"/>
-      <c r="CV13" s="29"/>
-      <c r="CW13" s="29"/>
-      <c r="CX13" s="29"/>
-      <c r="CY13" s="29"/>
-      <c r="CZ13" s="29"/>
-      <c r="DA13" s="29"/>
-      <c r="DB13" s="29"/>
-      <c r="DC13" s="29"/>
-      <c r="DD13" s="29"/>
-      <c r="DE13" s="29"/>
-      <c r="DF13" s="29"/>
-      <c r="DG13" s="29"/>
-      <c r="DH13" s="29"/>
-      <c r="DI13" s="29"/>
-      <c r="DJ13" s="29"/>
-      <c r="DK13" s="29"/>
-      <c r="DL13" s="29"/>
-      <c r="DM13" s="29"/>
-      <c r="DN13" s="29"/>
-      <c r="DO13" s="29"/>
-      <c r="DP13" s="29"/>
+      <c r="CV13"/>
+      <c r="CW13"/>
+      <c r="CX13"/>
+      <c r="CY13"/>
+      <c r="CZ13"/>
+      <c r="DA13"/>
+      <c r="DB13"/>
+      <c r="DC13"/>
+      <c r="DD13"/>
+      <c r="DE13"/>
+      <c r="DF13"/>
+      <c r="DG13"/>
+      <c r="DH13"/>
+      <c r="DI13"/>
+      <c r="DJ13"/>
+      <c r="DK13"/>
+      <c r="DL13"/>
+      <c r="DM13"/>
+      <c r="DN13"/>
+      <c r="DO13"/>
+      <c r="DP13"/>
     </row>
     <row r="14" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="43" t="s">
@@ -4001,7 +3782,7 @@
       <c r="F14" s="75"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I14" s="29"/>
@@ -4095,27 +3876,27 @@
       <c r="CS14" s="29"/>
       <c r="CT14" s="29"/>
       <c r="CU14" s="29"/>
-      <c r="CV14" s="29"/>
-      <c r="CW14" s="29"/>
-      <c r="CX14" s="29"/>
-      <c r="CY14" s="29"/>
-      <c r="CZ14" s="29"/>
-      <c r="DA14" s="29"/>
-      <c r="DB14" s="29"/>
-      <c r="DC14" s="29"/>
-      <c r="DD14" s="29"/>
-      <c r="DE14" s="29"/>
-      <c r="DF14" s="29"/>
-      <c r="DG14" s="29"/>
-      <c r="DH14" s="29"/>
-      <c r="DI14" s="29"/>
-      <c r="DJ14" s="29"/>
-      <c r="DK14" s="29"/>
-      <c r="DL14" s="29"/>
-      <c r="DM14" s="29"/>
-      <c r="DN14" s="29"/>
-      <c r="DO14" s="29"/>
-      <c r="DP14" s="29"/>
+      <c r="CV14"/>
+      <c r="CW14"/>
+      <c r="CX14"/>
+      <c r="CY14"/>
+      <c r="CZ14"/>
+      <c r="DA14"/>
+      <c r="DB14"/>
+      <c r="DC14"/>
+      <c r="DD14"/>
+      <c r="DE14"/>
+      <c r="DF14"/>
+      <c r="DG14"/>
+      <c r="DH14"/>
+      <c r="DI14"/>
+      <c r="DJ14"/>
+      <c r="DK14"/>
+      <c r="DL14"/>
+      <c r="DM14"/>
+      <c r="DN14"/>
+      <c r="DO14"/>
+      <c r="DP14"/>
     </row>
     <row r="15" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="43"/>
@@ -4128,7 +3909,7 @@
       <c r="F15" s="77"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I15" s="29"/>
@@ -4222,27 +4003,27 @@
       <c r="CS15" s="29"/>
       <c r="CT15" s="29"/>
       <c r="CU15" s="29"/>
-      <c r="CV15" s="29"/>
-      <c r="CW15" s="29"/>
-      <c r="CX15" s="29"/>
-      <c r="CY15" s="29"/>
-      <c r="CZ15" s="29"/>
-      <c r="DA15" s="29"/>
-      <c r="DB15" s="29"/>
-      <c r="DC15" s="29"/>
-      <c r="DD15" s="29"/>
-      <c r="DE15" s="29"/>
-      <c r="DF15" s="29"/>
-      <c r="DG15" s="29"/>
-      <c r="DH15" s="29"/>
-      <c r="DI15" s="29"/>
-      <c r="DJ15" s="29"/>
-      <c r="DK15" s="29"/>
-      <c r="DL15" s="29"/>
-      <c r="DM15" s="29"/>
-      <c r="DN15" s="29"/>
-      <c r="DO15" s="29"/>
-      <c r="DP15" s="29"/>
+      <c r="CV15"/>
+      <c r="CW15"/>
+      <c r="CX15"/>
+      <c r="CY15"/>
+      <c r="CZ15"/>
+      <c r="DA15"/>
+      <c r="DB15"/>
+      <c r="DC15"/>
+      <c r="DD15"/>
+      <c r="DE15"/>
+      <c r="DF15"/>
+      <c r="DG15"/>
+      <c r="DH15"/>
+      <c r="DI15"/>
+      <c r="DJ15"/>
+      <c r="DK15"/>
+      <c r="DL15"/>
+      <c r="DM15"/>
+      <c r="DN15"/>
+      <c r="DO15"/>
+      <c r="DP15"/>
     </row>
     <row r="16" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="42"/>
@@ -4261,7 +4042,7 @@
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>16</v>
       </c>
       <c r="I16" s="29"/>
@@ -4355,27 +4136,27 @@
       <c r="CS16" s="29"/>
       <c r="CT16" s="29"/>
       <c r="CU16" s="29"/>
-      <c r="CV16" s="29"/>
-      <c r="CW16" s="29"/>
-      <c r="CX16" s="29"/>
-      <c r="CY16" s="29"/>
-      <c r="CZ16" s="29"/>
-      <c r="DA16" s="29"/>
-      <c r="DB16" s="29"/>
-      <c r="DC16" s="29"/>
-      <c r="DD16" s="29"/>
-      <c r="DE16" s="29"/>
-      <c r="DF16" s="29"/>
-      <c r="DG16" s="29"/>
-      <c r="DH16" s="29"/>
-      <c r="DI16" s="29"/>
-      <c r="DJ16" s="29"/>
-      <c r="DK16" s="29"/>
-      <c r="DL16" s="29"/>
-      <c r="DM16" s="29"/>
-      <c r="DN16" s="29"/>
-      <c r="DO16" s="29"/>
-      <c r="DP16" s="29"/>
+      <c r="CV16"/>
+      <c r="CW16"/>
+      <c r="CX16"/>
+      <c r="CY16"/>
+      <c r="CZ16"/>
+      <c r="DA16"/>
+      <c r="DB16"/>
+      <c r="DC16"/>
+      <c r="DD16"/>
+      <c r="DE16"/>
+      <c r="DF16"/>
+      <c r="DG16"/>
+      <c r="DH16"/>
+      <c r="DI16"/>
+      <c r="DJ16"/>
+      <c r="DK16"/>
+      <c r="DL16"/>
+      <c r="DM16"/>
+      <c r="DN16"/>
+      <c r="DO16"/>
+      <c r="DP16"/>
     </row>
     <row r="17" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="42"/>
@@ -4394,7 +4175,7 @@
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>21</v>
       </c>
       <c r="I17" s="29"/>
@@ -4488,27 +4269,27 @@
       <c r="CS17" s="29"/>
       <c r="CT17" s="29"/>
       <c r="CU17" s="29"/>
-      <c r="CV17" s="29"/>
-      <c r="CW17" s="29"/>
-      <c r="CX17" s="29"/>
-      <c r="CY17" s="29"/>
-      <c r="CZ17" s="29"/>
-      <c r="DA17" s="29"/>
-      <c r="DB17" s="29"/>
-      <c r="DC17" s="29"/>
-      <c r="DD17" s="29"/>
-      <c r="DE17" s="29"/>
-      <c r="DF17" s="29"/>
-      <c r="DG17" s="29"/>
-      <c r="DH17" s="29"/>
-      <c r="DI17" s="29"/>
-      <c r="DJ17" s="29"/>
-      <c r="DK17" s="29"/>
-      <c r="DL17" s="29"/>
-      <c r="DM17" s="29"/>
-      <c r="DN17" s="29"/>
-      <c r="DO17" s="29"/>
-      <c r="DP17" s="29"/>
+      <c r="CV17"/>
+      <c r="CW17"/>
+      <c r="CX17"/>
+      <c r="CY17"/>
+      <c r="CZ17"/>
+      <c r="DA17"/>
+      <c r="DB17"/>
+      <c r="DC17"/>
+      <c r="DD17"/>
+      <c r="DE17"/>
+      <c r="DF17"/>
+      <c r="DG17"/>
+      <c r="DH17"/>
+      <c r="DI17"/>
+      <c r="DJ17"/>
+      <c r="DK17"/>
+      <c r="DL17"/>
+      <c r="DM17"/>
+      <c r="DN17"/>
+      <c r="DO17"/>
+      <c r="DP17"/>
     </row>
     <row r="18" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="42"/>
@@ -4521,7 +4302,7 @@
       <c r="F18" s="77"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I18" s="29"/>
@@ -4615,27 +4396,27 @@
       <c r="CS18" s="29"/>
       <c r="CT18" s="29"/>
       <c r="CU18" s="29"/>
-      <c r="CV18" s="29"/>
-      <c r="CW18" s="29"/>
-      <c r="CX18" s="29"/>
-      <c r="CY18" s="29"/>
-      <c r="CZ18" s="29"/>
-      <c r="DA18" s="29"/>
-      <c r="DB18" s="29"/>
-      <c r="DC18" s="29"/>
-      <c r="DD18" s="29"/>
-      <c r="DE18" s="29"/>
-      <c r="DF18" s="29"/>
-      <c r="DG18" s="29"/>
-      <c r="DH18" s="29"/>
-      <c r="DI18" s="29"/>
-      <c r="DJ18" s="29"/>
-      <c r="DK18" s="29"/>
-      <c r="DL18" s="29"/>
-      <c r="DM18" s="29"/>
-      <c r="DN18" s="29"/>
-      <c r="DO18" s="29"/>
-      <c r="DP18" s="29"/>
+      <c r="CV18"/>
+      <c r="CW18"/>
+      <c r="CX18"/>
+      <c r="CY18"/>
+      <c r="CZ18"/>
+      <c r="DA18"/>
+      <c r="DB18"/>
+      <c r="DC18"/>
+      <c r="DD18"/>
+      <c r="DE18"/>
+      <c r="DF18"/>
+      <c r="DG18"/>
+      <c r="DH18"/>
+      <c r="DI18"/>
+      <c r="DJ18"/>
+      <c r="DK18"/>
+      <c r="DL18"/>
+      <c r="DM18"/>
+      <c r="DN18"/>
+      <c r="DO18"/>
+      <c r="DP18"/>
     </row>
     <row r="19" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="42"/>
@@ -4654,7 +4435,7 @@
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>31</v>
       </c>
       <c r="I19" s="29"/>
@@ -4748,27 +4529,27 @@
       <c r="CS19" s="29"/>
       <c r="CT19" s="29"/>
       <c r="CU19" s="29"/>
-      <c r="CV19" s="29"/>
-      <c r="CW19" s="29"/>
-      <c r="CX19" s="29"/>
-      <c r="CY19" s="29"/>
-      <c r="CZ19" s="29"/>
-      <c r="DA19" s="29"/>
-      <c r="DB19" s="29"/>
-      <c r="DC19" s="29"/>
-      <c r="DD19" s="29"/>
-      <c r="DE19" s="29"/>
-      <c r="DF19" s="29"/>
-      <c r="DG19" s="29"/>
-      <c r="DH19" s="29"/>
-      <c r="DI19" s="29"/>
-      <c r="DJ19" s="29"/>
-      <c r="DK19" s="29"/>
-      <c r="DL19" s="29"/>
-      <c r="DM19" s="29"/>
-      <c r="DN19" s="29"/>
-      <c r="DO19" s="29"/>
-      <c r="DP19" s="29"/>
+      <c r="CV19"/>
+      <c r="CW19"/>
+      <c r="CX19"/>
+      <c r="CY19"/>
+      <c r="CZ19"/>
+      <c r="DA19"/>
+      <c r="DB19"/>
+      <c r="DC19"/>
+      <c r="DD19"/>
+      <c r="DE19"/>
+      <c r="DF19"/>
+      <c r="DG19"/>
+      <c r="DH19"/>
+      <c r="DI19"/>
+      <c r="DJ19"/>
+      <c r="DK19"/>
+      <c r="DL19"/>
+      <c r="DM19"/>
+      <c r="DN19"/>
+      <c r="DO19"/>
+      <c r="DP19"/>
     </row>
     <row r="20" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
@@ -4783,7 +4564,7 @@
       <c r="F20" s="77"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I20" s="29"/>
@@ -4877,27 +4658,27 @@
       <c r="CS20" s="29"/>
       <c r="CT20" s="29"/>
       <c r="CU20" s="29"/>
-      <c r="CV20" s="29"/>
-      <c r="CW20" s="29"/>
-      <c r="CX20" s="29"/>
-      <c r="CY20" s="29"/>
-      <c r="CZ20" s="29"/>
-      <c r="DA20" s="29"/>
-      <c r="DB20" s="29"/>
-      <c r="DC20" s="29"/>
-      <c r="DD20" s="29"/>
-      <c r="DE20" s="29"/>
-      <c r="DF20" s="29"/>
-      <c r="DG20" s="29"/>
-      <c r="DH20" s="29"/>
-      <c r="DI20" s="29"/>
-      <c r="DJ20" s="29"/>
-      <c r="DK20" s="29"/>
-      <c r="DL20" s="29"/>
-      <c r="DM20" s="29"/>
-      <c r="DN20" s="29"/>
-      <c r="DO20" s="29"/>
-      <c r="DP20" s="29"/>
+      <c r="CV20"/>
+      <c r="CW20"/>
+      <c r="CX20"/>
+      <c r="CY20"/>
+      <c r="CZ20"/>
+      <c r="DA20"/>
+      <c r="DB20"/>
+      <c r="DC20"/>
+      <c r="DD20"/>
+      <c r="DE20"/>
+      <c r="DF20"/>
+      <c r="DG20"/>
+      <c r="DH20"/>
+      <c r="DI20"/>
+      <c r="DJ20"/>
+      <c r="DK20"/>
+      <c r="DL20"/>
+      <c r="DM20"/>
+      <c r="DN20"/>
+      <c r="DO20"/>
+      <c r="DP20"/>
     </row>
     <row r="21" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="42"/>
@@ -4916,7 +4697,7 @@
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>21</v>
       </c>
       <c r="I21" s="29"/>
@@ -5010,27 +4791,27 @@
       <c r="CS21" s="29"/>
       <c r="CT21" s="29"/>
       <c r="CU21" s="29"/>
-      <c r="CV21" s="29"/>
-      <c r="CW21" s="29"/>
-      <c r="CX21" s="29"/>
-      <c r="CY21" s="29"/>
-      <c r="CZ21" s="29"/>
-      <c r="DA21" s="29"/>
-      <c r="DB21" s="29"/>
-      <c r="DC21" s="29"/>
-      <c r="DD21" s="29"/>
-      <c r="DE21" s="29"/>
-      <c r="DF21" s="29"/>
-      <c r="DG21" s="29"/>
-      <c r="DH21" s="29"/>
-      <c r="DI21" s="29"/>
-      <c r="DJ21" s="29"/>
-      <c r="DK21" s="29"/>
-      <c r="DL21" s="29"/>
-      <c r="DM21" s="29"/>
-      <c r="DN21" s="29"/>
-      <c r="DO21" s="29"/>
-      <c r="DP21" s="29"/>
+      <c r="CV21"/>
+      <c r="CW21"/>
+      <c r="CX21"/>
+      <c r="CY21"/>
+      <c r="CZ21"/>
+      <c r="DA21"/>
+      <c r="DB21"/>
+      <c r="DC21"/>
+      <c r="DD21"/>
+      <c r="DE21"/>
+      <c r="DF21"/>
+      <c r="DG21"/>
+      <c r="DH21"/>
+      <c r="DI21"/>
+      <c r="DJ21"/>
+      <c r="DK21"/>
+      <c r="DL21"/>
+      <c r="DM21"/>
+      <c r="DN21"/>
+      <c r="DO21"/>
+      <c r="DP21"/>
     </row>
     <row r="22" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="42"/>
@@ -5049,7 +4830,7 @@
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>31</v>
       </c>
       <c r="I22" s="29"/>
@@ -5143,27 +4924,27 @@
       <c r="CS22" s="29"/>
       <c r="CT22" s="29"/>
       <c r="CU22" s="29"/>
-      <c r="CV22" s="29"/>
-      <c r="CW22" s="29"/>
-      <c r="CX22" s="29"/>
-      <c r="CY22" s="29"/>
-      <c r="CZ22" s="29"/>
-      <c r="DA22" s="29"/>
-      <c r="DB22" s="29"/>
-      <c r="DC22" s="29"/>
-      <c r="DD22" s="29"/>
-      <c r="DE22" s="29"/>
-      <c r="DF22" s="29"/>
-      <c r="DG22" s="29"/>
-      <c r="DH22" s="29"/>
-      <c r="DI22" s="29"/>
-      <c r="DJ22" s="29"/>
-      <c r="DK22" s="29"/>
-      <c r="DL22" s="29"/>
-      <c r="DM22" s="29"/>
-      <c r="DN22" s="29"/>
-      <c r="DO22" s="29"/>
-      <c r="DP22" s="29"/>
+      <c r="CV22"/>
+      <c r="CW22"/>
+      <c r="CX22"/>
+      <c r="CY22"/>
+      <c r="CZ22"/>
+      <c r="DA22"/>
+      <c r="DB22"/>
+      <c r="DC22"/>
+      <c r="DD22"/>
+      <c r="DE22"/>
+      <c r="DF22"/>
+      <c r="DG22"/>
+      <c r="DH22"/>
+      <c r="DI22"/>
+      <c r="DJ22"/>
+      <c r="DK22"/>
+      <c r="DL22"/>
+      <c r="DM22"/>
+      <c r="DN22"/>
+      <c r="DO22"/>
+      <c r="DP22"/>
     </row>
     <row r="23" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="42"/>
@@ -5182,7 +4963,7 @@
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>36</v>
       </c>
       <c r="I23" s="29"/>
@@ -5276,27 +5057,27 @@
       <c r="CS23" s="29"/>
       <c r="CT23" s="29"/>
       <c r="CU23" s="29"/>
-      <c r="CV23" s="29"/>
-      <c r="CW23" s="29"/>
-      <c r="CX23" s="29"/>
-      <c r="CY23" s="29"/>
-      <c r="CZ23" s="29"/>
-      <c r="DA23" s="29"/>
-      <c r="DB23" s="29"/>
-      <c r="DC23" s="29"/>
-      <c r="DD23" s="29"/>
-      <c r="DE23" s="29"/>
-      <c r="DF23" s="29"/>
-      <c r="DG23" s="29"/>
-      <c r="DH23" s="29"/>
-      <c r="DI23" s="29"/>
-      <c r="DJ23" s="29"/>
-      <c r="DK23" s="29"/>
-      <c r="DL23" s="29"/>
-      <c r="DM23" s="29"/>
-      <c r="DN23" s="29"/>
-      <c r="DO23" s="29"/>
-      <c r="DP23" s="29"/>
+      <c r="CV23"/>
+      <c r="CW23"/>
+      <c r="CX23"/>
+      <c r="CY23"/>
+      <c r="CZ23"/>
+      <c r="DA23"/>
+      <c r="DB23"/>
+      <c r="DC23"/>
+      <c r="DD23"/>
+      <c r="DE23"/>
+      <c r="DF23"/>
+      <c r="DG23"/>
+      <c r="DH23"/>
+      <c r="DI23"/>
+      <c r="DJ23"/>
+      <c r="DK23"/>
+      <c r="DL23"/>
+      <c r="DM23"/>
+      <c r="DN23"/>
+      <c r="DO23"/>
+      <c r="DP23"/>
     </row>
     <row r="24" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="42"/>
@@ -5309,7 +5090,7 @@
       <c r="F24" s="27"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I24" s="29"/>
@@ -5403,27 +5184,27 @@
       <c r="CS24" s="29"/>
       <c r="CT24" s="29"/>
       <c r="CU24" s="29"/>
-      <c r="CV24" s="29"/>
-      <c r="CW24" s="29"/>
-      <c r="CX24" s="29"/>
-      <c r="CY24" s="29"/>
-      <c r="CZ24" s="29"/>
-      <c r="DA24" s="29"/>
-      <c r="DB24" s="29"/>
-      <c r="DC24" s="29"/>
-      <c r="DD24" s="29"/>
-      <c r="DE24" s="29"/>
-      <c r="DF24" s="29"/>
-      <c r="DG24" s="29"/>
-      <c r="DH24" s="29"/>
-      <c r="DI24" s="29"/>
-      <c r="DJ24" s="29"/>
-      <c r="DK24" s="29"/>
-      <c r="DL24" s="29"/>
-      <c r="DM24" s="29"/>
-      <c r="DN24" s="29"/>
-      <c r="DO24" s="29"/>
-      <c r="DP24" s="29"/>
+      <c r="CV24"/>
+      <c r="CW24"/>
+      <c r="CX24"/>
+      <c r="CY24"/>
+      <c r="CZ24"/>
+      <c r="DA24"/>
+      <c r="DB24"/>
+      <c r="DC24"/>
+      <c r="DD24"/>
+      <c r="DE24"/>
+      <c r="DF24"/>
+      <c r="DG24"/>
+      <c r="DH24"/>
+      <c r="DI24"/>
+      <c r="DJ24"/>
+      <c r="DK24"/>
+      <c r="DL24"/>
+      <c r="DM24"/>
+      <c r="DN24"/>
+      <c r="DO24"/>
+      <c r="DP24"/>
     </row>
     <row r="25" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="42"/>
@@ -5434,15 +5215,15 @@
       <c r="D25" s="28"/>
       <c r="E25" s="51">
         <f ca="1">E3+78</f>
-        <v>44921</v>
+        <v>44922</v>
       </c>
       <c r="F25" s="51">
         <f ca="1">E3+89</f>
-        <v>44932</v>
+        <v>44933</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="32"/>
         <v>12</v>
       </c>
       <c r="I25" s="29"/>
@@ -5536,27 +5317,27 @@
       <c r="CS25" s="29"/>
       <c r="CT25" s="29"/>
       <c r="CU25" s="29"/>
-      <c r="CV25" s="29"/>
-      <c r="CW25" s="29"/>
-      <c r="CX25" s="29"/>
-      <c r="CY25" s="29"/>
-      <c r="CZ25" s="29"/>
-      <c r="DA25" s="29"/>
-      <c r="DB25" s="29"/>
-      <c r="DC25" s="29"/>
-      <c r="DD25" s="29"/>
-      <c r="DE25" s="29"/>
-      <c r="DF25" s="29"/>
-      <c r="DG25" s="29"/>
-      <c r="DH25" s="29"/>
-      <c r="DI25" s="29"/>
-      <c r="DJ25" s="29"/>
-      <c r="DK25" s="29"/>
-      <c r="DL25" s="29"/>
-      <c r="DM25" s="29"/>
-      <c r="DN25" s="29"/>
-      <c r="DO25" s="29"/>
-      <c r="DP25" s="29"/>
+      <c r="CV25"/>
+      <c r="CW25"/>
+      <c r="CX25"/>
+      <c r="CY25"/>
+      <c r="CZ25"/>
+      <c r="DA25"/>
+      <c r="DB25"/>
+      <c r="DC25"/>
+      <c r="DD25"/>
+      <c r="DE25"/>
+      <c r="DF25"/>
+      <c r="DG25"/>
+      <c r="DH25"/>
+      <c r="DI25"/>
+      <c r="DJ25"/>
+      <c r="DK25"/>
+      <c r="DL25"/>
+      <c r="DM25"/>
+      <c r="DN25"/>
+      <c r="DO25"/>
+      <c r="DP25"/>
     </row>
     <row r="26" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="42" t="s">
@@ -5599,10 +5380,7 @@
       <c r="C36" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
+  <mergeCells count="16">
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="CA4:CG4"/>
@@ -5754,45 +5532,6 @@
       <formula>AND(task_end&gt;=CO$5,task_start&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CV5:DB25">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>AND(TODAY()&gt;=CV$5,TODAY()&lt;CW$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CV7:DB25">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>AND(task_start&lt;=CV$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CV$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
-      <formula>AND(task_end&gt;=CV$5,task_start&lt;CW$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DC5:DI25">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>AND(TODAY()&gt;=DC$5,TODAY()&lt;DD$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DC7:DI25">
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>AND(task_start&lt;=DC$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=DC$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
-      <formula>AND(task_end&gt;=DC$5,task_start&lt;DD$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DJ5:DP25">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>AND(TODAY()&gt;=DJ$5,TODAY()&lt;DK$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DJ7:DP25">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND(task_start&lt;=DJ$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=DJ$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>AND(task_end&gt;=DJ$5,task_start&lt;DK$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
@@ -5800,7 +5539,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="35" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="41" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -5877,7 +5616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Gestion de projet - modif gantt.jpeg and xlsx
</commit_message>
<xml_diff>
--- a/doc/livrable_1/rapport/templates/gantt.xlsx
+++ b/doc/livrable_1/rapport/templates/gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{C9655527-7F3E-417B-AA5C-08656AAAE3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE18601-98C6-4A39-B78A-8A8726E2B84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Project Start:</t>
   </si>
@@ -219,22 +219,10 @@
     <t xml:space="preserve">   Conception des requêtes</t>
   </si>
   <si>
-    <t>Python (Flask)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Partie serveur</t>
-  </si>
-  <si>
-    <t>Partie client</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Next/React</t>
   </si>
   <si>
     <t xml:space="preserve">   CSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   HTML</t>
   </si>
   <si>
     <t>Rendu final</t>
@@ -244,6 +232,27 @@
   </si>
   <si>
     <t>NOTRE PROJET</t>
+  </si>
+  <si>
+    <t>Base de données</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Algorithmique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Flask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Réception/Émission en JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   JSX</t>
   </si>
 </sst>
 </file>
@@ -639,7 +648,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -817,50 +826,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="11" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="7" borderId="2" xfId="10" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="11" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="7" borderId="2" xfId="10" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -878,307 +881,7 @@
     <cellStyle name="Titre 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <fill>
         <patternFill>
@@ -1485,15 +1188,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="59"/>
-      <tableStyleElement type="headerRow" dxfId="58"/>
-      <tableStyleElement type="totalRow" dxfId="57"/>
-      <tableStyleElement type="firstColumn" dxfId="56"/>
-      <tableStyleElement type="lastColumn" dxfId="55"/>
-      <tableStyleElement type="firstRowStripe" dxfId="54"/>
-      <tableStyleElement type="secondRowStripe" dxfId="53"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="52"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="51"/>
+      <tableStyleElement type="wholeTable" dxfId="29"/>
+      <tableStyleElement type="headerRow" dxfId="28"/>
+      <tableStyleElement type="totalRow" dxfId="27"/>
+      <tableStyleElement type="firstColumn" dxfId="26"/>
+      <tableStyleElement type="lastColumn" dxfId="25"/>
+      <tableStyleElement type="firstRowStripe" dxfId="24"/>
+      <tableStyleElement type="secondRowStripe" dxfId="23"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="22"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="21"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1908,11 +1611,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DP36"/>
+  <dimension ref="A1:DP38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1933,7 +1636,7 @@
         <v>27</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1954,157 +1657,157 @@
         <v>34</v>
       </c>
       <c r="B3" s="48"/>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="70">
+      <c r="D3" s="77"/>
+      <c r="E3" s="75">
         <f ca="1">TODAY()-9</f>
         <v>44844</v>
       </c>
-      <c r="F3" s="70"/>
+      <c r="F3" s="75"/>
     </row>
     <row r="4" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="66"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="67">
+      <c r="I4" s="72">
         <f ca="1">I5</f>
         <v>44844</v>
       </c>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="67">
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="72">
         <f ca="1">P5</f>
         <v>44851</v>
       </c>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="68"/>
-      <c r="S4" s="68"/>
-      <c r="T4" s="68"/>
-      <c r="U4" s="68"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="67">
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="72">
         <f ca="1">W5</f>
         <v>44858</v>
       </c>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="68"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="68"/>
-      <c r="AB4" s="68"/>
-      <c r="AC4" s="69"/>
-      <c r="AD4" s="67">
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="73"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="72">
         <f ca="1">AD5</f>
         <v>44865</v>
       </c>
-      <c r="AE4" s="68"/>
-      <c r="AF4" s="68"/>
-      <c r="AG4" s="68"/>
-      <c r="AH4" s="68"/>
-      <c r="AI4" s="68"/>
-      <c r="AJ4" s="69"/>
-      <c r="AK4" s="67">
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
+      <c r="AG4" s="73"/>
+      <c r="AH4" s="73"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="74"/>
+      <c r="AK4" s="72">
         <f ca="1">AK5</f>
         <v>44872</v>
       </c>
-      <c r="AL4" s="68"/>
-      <c r="AM4" s="68"/>
-      <c r="AN4" s="68"/>
-      <c r="AO4" s="68"/>
-      <c r="AP4" s="68"/>
-      <c r="AQ4" s="69"/>
-      <c r="AR4" s="67">
+      <c r="AL4" s="73"/>
+      <c r="AM4" s="73"/>
+      <c r="AN4" s="73"/>
+      <c r="AO4" s="73"/>
+      <c r="AP4" s="73"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="72">
         <f ca="1">AR5</f>
         <v>44879</v>
       </c>
-      <c r="AS4" s="68"/>
-      <c r="AT4" s="68"/>
-      <c r="AU4" s="68"/>
-      <c r="AV4" s="68"/>
-      <c r="AW4" s="68"/>
-      <c r="AX4" s="69"/>
-      <c r="AY4" s="67">
+      <c r="AS4" s="73"/>
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
+      <c r="AW4" s="73"/>
+      <c r="AX4" s="74"/>
+      <c r="AY4" s="72">
         <f ca="1">AY5</f>
         <v>44886</v>
       </c>
-      <c r="AZ4" s="68"/>
-      <c r="BA4" s="68"/>
-      <c r="BB4" s="68"/>
-      <c r="BC4" s="68"/>
-      <c r="BD4" s="68"/>
-      <c r="BE4" s="69"/>
-      <c r="BF4" s="67">
+      <c r="AZ4" s="73"/>
+      <c r="BA4" s="73"/>
+      <c r="BB4" s="73"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="73"/>
+      <c r="BE4" s="74"/>
+      <c r="BF4" s="72">
         <f ca="1">BF5</f>
         <v>44893</v>
       </c>
-      <c r="BG4" s="68"/>
-      <c r="BH4" s="68"/>
-      <c r="BI4" s="68"/>
-      <c r="BJ4" s="68"/>
-      <c r="BK4" s="68"/>
-      <c r="BL4" s="69"/>
-      <c r="BM4" s="67">
+      <c r="BG4" s="73"/>
+      <c r="BH4" s="73"/>
+      <c r="BI4" s="73"/>
+      <c r="BJ4" s="73"/>
+      <c r="BK4" s="73"/>
+      <c r="BL4" s="74"/>
+      <c r="BM4" s="72">
         <f ca="1">BM5</f>
         <v>44900</v>
       </c>
-      <c r="BN4" s="68"/>
-      <c r="BO4" s="68"/>
-      <c r="BP4" s="68"/>
-      <c r="BQ4" s="68"/>
-      <c r="BR4" s="68"/>
-      <c r="BS4" s="69"/>
-      <c r="BT4" s="67">
+      <c r="BN4" s="73"/>
+      <c r="BO4" s="73"/>
+      <c r="BP4" s="73"/>
+      <c r="BQ4" s="73"/>
+      <c r="BR4" s="73"/>
+      <c r="BS4" s="74"/>
+      <c r="BT4" s="72">
         <f ca="1">BT5</f>
         <v>44907</v>
       </c>
-      <c r="BU4" s="68"/>
-      <c r="BV4" s="68"/>
-      <c r="BW4" s="68"/>
-      <c r="BX4" s="68"/>
-      <c r="BY4" s="68"/>
-      <c r="BZ4" s="69"/>
-      <c r="CA4" s="67">
+      <c r="BU4" s="73"/>
+      <c r="BV4" s="73"/>
+      <c r="BW4" s="73"/>
+      <c r="BX4" s="73"/>
+      <c r="BY4" s="73"/>
+      <c r="BZ4" s="74"/>
+      <c r="CA4" s="72">
         <f ca="1">CA5</f>
         <v>44914</v>
       </c>
-      <c r="CB4" s="68"/>
-      <c r="CC4" s="68"/>
-      <c r="CD4" s="68"/>
-      <c r="CE4" s="68"/>
-      <c r="CF4" s="68"/>
-      <c r="CG4" s="69"/>
-      <c r="CH4" s="67">
+      <c r="CB4" s="73"/>
+      <c r="CC4" s="73"/>
+      <c r="CD4" s="73"/>
+      <c r="CE4" s="73"/>
+      <c r="CF4" s="73"/>
+      <c r="CG4" s="74"/>
+      <c r="CH4" s="72">
         <f ca="1">CH5</f>
         <v>44921</v>
       </c>
-      <c r="CI4" s="68"/>
-      <c r="CJ4" s="68"/>
-      <c r="CK4" s="68"/>
-      <c r="CL4" s="68"/>
-      <c r="CM4" s="68"/>
-      <c r="CN4" s="69"/>
-      <c r="CO4" s="67">
+      <c r="CI4" s="73"/>
+      <c r="CJ4" s="73"/>
+      <c r="CK4" s="73"/>
+      <c r="CL4" s="73"/>
+      <c r="CM4" s="73"/>
+      <c r="CN4" s="74"/>
+      <c r="CO4" s="72">
         <f ca="1">CO5</f>
         <v>44928</v>
       </c>
-      <c r="CP4" s="68"/>
-      <c r="CQ4" s="68"/>
-      <c r="CR4" s="68"/>
-      <c r="CS4" s="68"/>
-      <c r="CT4" s="68"/>
-      <c r="CU4" s="69"/>
+      <c r="CP4" s="73"/>
+      <c r="CQ4" s="73"/>
+      <c r="CR4" s="73"/>
+      <c r="CS4" s="73"/>
+      <c r="CT4" s="73"/>
+      <c r="CU4" s="74"/>
     </row>
     <row r="5" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
@@ -2729,7 +2432,7 @@
         <v>d</v>
       </c>
       <c r="BM6" s="13" t="str">
-        <f t="shared" ref="BM6:DP6" ca="1" si="31">LEFT(TEXT(BM5,"ddd"),1)</f>
+        <f t="shared" ref="BM6:CU6" ca="1" si="31">LEFT(TEXT(BM5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="BN6" s="13" t="str">
@@ -2984,7 +2687,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="str">
-        <f t="shared" ref="H8:H25" si="32">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H27" si="32">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="29"/>
@@ -3773,13 +3476,13 @@
       <c r="A14" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="72"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="75"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="69"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16" t="str">
         <f t="shared" si="32"/>
@@ -3900,13 +3603,13 @@
     </row>
     <row r="15" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="43"/>
-      <c r="B15" s="78" t="s">
-        <v>43</v>
+      <c r="B15" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="C15" s="54"/>
       <c r="D15" s="22"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16" t="str">
         <f t="shared" si="32"/>
@@ -4293,13 +3996,13 @@
     </row>
     <row r="18" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="42"/>
-      <c r="B18" s="76" t="s">
-        <v>46</v>
+      <c r="B18" s="71" t="s">
+        <v>53</v>
       </c>
       <c r="C18" s="54"/>
       <c r="D18" s="22"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16" t="str">
         <f t="shared" si="32"/>
@@ -4421,23 +4124,20 @@
     <row r="19" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="42"/>
       <c r="B19" s="59" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C19" s="55"/>
       <c r="D19" s="23"/>
       <c r="E19" s="50">
-        <f ca="1">E17</f>
-        <v>44871</v>
+        <f ca="1">F13</f>
+        <v>44856</v>
       </c>
       <c r="F19" s="50">
         <f ca="1">E19+30</f>
-        <v>44901</v>
+        <v>44886</v>
       </c>
       <c r="G19" s="16"/>
-      <c r="H19" s="16">
-        <f t="shared" ca="1" si="32"/>
-        <v>31</v>
-      </c>
+      <c r="H19" s="16"/>
       <c r="I19" s="29"/>
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
@@ -4454,7 +4154,7 @@
       <c r="V19" s="29"/>
       <c r="W19" s="29"/>
       <c r="X19" s="29"/>
-      <c r="Y19" s="29"/>
+      <c r="Y19" s="30"/>
       <c r="Z19" s="29"/>
       <c r="AA19" s="29"/>
       <c r="AB19" s="29"/>
@@ -4552,21 +4252,22 @@
       <c r="DP19"/>
     </row>
     <row r="20" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="50">
+        <f ca="1">F19-15</f>
+        <v>44871</v>
+      </c>
+      <c r="F20" s="50">
+        <f ca="1">E20+30</f>
+        <v>44901</v>
+      </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="16" t="str">
-        <f t="shared" si="32"/>
-        <v/>
-      </c>
+      <c r="H20" s="16"/>
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
@@ -4583,7 +4284,7 @@
       <c r="V20" s="29"/>
       <c r="W20" s="29"/>
       <c r="X20" s="29"/>
-      <c r="Y20" s="29"/>
+      <c r="Y20" s="30"/>
       <c r="Z20" s="29"/>
       <c r="AA20" s="29"/>
       <c r="AB20" s="29"/>
@@ -4683,22 +4384,22 @@
     <row r="21" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="42"/>
       <c r="B21" s="59" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C21" s="55"/>
       <c r="D21" s="23"/>
       <c r="E21" s="50">
-        <f ca="1">E17</f>
-        <v>44871</v>
+        <f ca="1">E25+10</f>
+        <v>44891</v>
       </c>
       <c r="F21" s="50">
-        <f ca="1">E21+20</f>
-        <v>44891</v>
+        <f ca="1">E21+25</f>
+        <v>44916</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="16">
         <f t="shared" ca="1" si="32"/>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
@@ -4814,24 +4515,20 @@
       <c r="DP21"/>
     </row>
     <row r="22" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="42"/>
-      <c r="B22" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="50">
-        <f ca="1">F21-15</f>
-        <v>44876</v>
-      </c>
-      <c r="F22" s="50">
-        <f ca="1">E22+30</f>
-        <v>44906</v>
-      </c>
+      <c r="A22" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="54"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
       <c r="G22" s="16"/>
-      <c r="H22" s="16">
-        <f t="shared" ca="1" si="32"/>
-        <v>31</v>
+      <c r="H22" s="16" t="str">
+        <f t="shared" si="32"/>
+        <v/>
       </c>
       <c r="I22" s="29"/>
       <c r="J22" s="29"/>
@@ -4949,22 +4646,22 @@
     <row r="23" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="42"/>
       <c r="B23" s="59" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C23" s="55"/>
       <c r="D23" s="23"/>
       <c r="E23" s="50">
-        <f ca="1">E22+5</f>
-        <v>44881</v>
+        <f ca="1">E17</f>
+        <v>44871</v>
       </c>
       <c r="F23" s="50">
-        <f ca="1">E23+35</f>
-        <v>44916</v>
+        <f ca="1">E23+20</f>
+        <v>44891</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="16">
         <f t="shared" ca="1" si="32"/>
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="I23" s="29"/>
       <c r="J23" s="29"/>
@@ -5081,17 +4778,23 @@
     </row>
     <row r="24" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="42"/>
-      <c r="B24" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="27"/>
+      <c r="B24" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="55"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="50">
+        <f ca="1">F23-15</f>
+        <v>44876</v>
+      </c>
+      <c r="F24" s="50">
+        <f ca="1">E24+30</f>
+        <v>44906</v>
+      </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="16" t="str">
-        <f t="shared" si="32"/>
-        <v/>
+      <c r="H24" s="16">
+        <f t="shared" ca="1" si="32"/>
+        <v>31</v>
       </c>
       <c r="I24" s="29"/>
       <c r="J24" s="29"/>
@@ -5208,23 +4911,23 @@
     </row>
     <row r="25" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="42"/>
-      <c r="B25" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="51">
-        <f ca="1">E3+78</f>
-        <v>44922</v>
-      </c>
-      <c r="F25" s="51">
-        <f ca="1">E3+89</f>
-        <v>44933</v>
+      <c r="B25" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="55"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="50">
+        <f ca="1">E24+5</f>
+        <v>44881</v>
+      </c>
+      <c r="F25" s="50">
+        <f ca="1">E25+35</f>
+        <v>44916</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16">
         <f t="shared" ca="1" si="32"/>
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
@@ -5339,16 +5042,270 @@
       <c r="DO25"/>
       <c r="DP25"/>
     </row>
-    <row r="26" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="42" t="s">
-        <v>24</v>
-      </c>
+    <row r="26" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="42"/>
+      <c r="B26" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="56"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="29"/>
+      <c r="AA26" s="29"/>
+      <c r="AB26" s="29"/>
+      <c r="AC26" s="29"/>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="29"/>
+      <c r="AF26" s="29"/>
+      <c r="AG26" s="29"/>
+      <c r="AH26" s="29"/>
+      <c r="AI26" s="29"/>
+      <c r="AJ26" s="29"/>
+      <c r="AK26" s="29"/>
+      <c r="AL26" s="29"/>
+      <c r="AM26" s="29"/>
+      <c r="AN26" s="29"/>
+      <c r="AO26" s="29"/>
+      <c r="AP26" s="29"/>
+      <c r="AQ26" s="29"/>
+      <c r="AR26" s="29"/>
+      <c r="AS26" s="29"/>
+      <c r="AT26" s="29"/>
+      <c r="AU26" s="29"/>
+      <c r="AV26" s="29"/>
+      <c r="AW26" s="29"/>
+      <c r="AX26" s="29"/>
+      <c r="AY26" s="29"/>
+      <c r="AZ26" s="29"/>
+      <c r="BA26" s="29"/>
+      <c r="BB26" s="29"/>
+      <c r="BC26" s="29"/>
+      <c r="BD26" s="29"/>
+      <c r="BE26" s="29"/>
+      <c r="BF26" s="29"/>
+      <c r="BG26" s="29"/>
+      <c r="BH26" s="29"/>
+      <c r="BI26" s="29"/>
+      <c r="BJ26" s="29"/>
+      <c r="BK26" s="29"/>
+      <c r="BL26" s="29"/>
+      <c r="BM26" s="29"/>
+      <c r="BN26" s="29"/>
+      <c r="BO26" s="29"/>
+      <c r="BP26" s="29"/>
+      <c r="BQ26" s="29"/>
+      <c r="BR26" s="29"/>
+      <c r="BS26" s="29"/>
+      <c r="BT26" s="29"/>
+      <c r="BU26" s="29"/>
+      <c r="BV26" s="29"/>
+      <c r="BW26" s="29"/>
+      <c r="BX26" s="29"/>
+      <c r="BY26" s="29"/>
+      <c r="BZ26" s="29"/>
+      <c r="CA26" s="29"/>
+      <c r="CB26" s="29"/>
+      <c r="CC26" s="29"/>
+      <c r="CD26" s="29"/>
+      <c r="CE26" s="29"/>
+      <c r="CF26" s="29"/>
+      <c r="CG26" s="29"/>
+      <c r="CH26" s="29"/>
+      <c r="CI26" s="29"/>
+      <c r="CJ26" s="29"/>
+      <c r="CK26" s="29"/>
+      <c r="CL26" s="29"/>
+      <c r="CM26" s="29"/>
+      <c r="CN26" s="29"/>
+      <c r="CO26" s="29"/>
+      <c r="CP26" s="29"/>
+      <c r="CQ26" s="29"/>
+      <c r="CR26" s="29"/>
+      <c r="CS26" s="29"/>
+      <c r="CT26" s="29"/>
+      <c r="CU26" s="29"/>
+      <c r="CV26"/>
+      <c r="CW26"/>
+      <c r="CX26"/>
+      <c r="CY26"/>
+      <c r="CZ26"/>
+      <c r="DA26"/>
+      <c r="DB26"/>
+      <c r="DC26"/>
+      <c r="DD26"/>
+      <c r="DE26"/>
+      <c r="DF26"/>
+      <c r="DG26"/>
+      <c r="DH26"/>
+      <c r="DI26"/>
+      <c r="DJ26"/>
+      <c r="DK26"/>
+      <c r="DL26"/>
+      <c r="DM26"/>
+      <c r="DN26"/>
+      <c r="DO26"/>
+      <c r="DP26"/>
     </row>
-    <row r="27" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="42"/>
+      <c r="B27" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="57"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="51">
+        <f ca="1">E3+78</f>
+        <v>44922</v>
+      </c>
+      <c r="F27" s="51">
+        <f ca="1">E3+89</f>
+        <v>44933</v>
+      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16">
+        <f t="shared" ca="1" si="32"/>
+        <v>12</v>
+      </c>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
+      <c r="AA27" s="29"/>
+      <c r="AB27" s="29"/>
+      <c r="AC27" s="29"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="29"/>
+      <c r="AG27" s="29"/>
+      <c r="AH27" s="29"/>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="29"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="29"/>
+      <c r="AM27" s="29"/>
+      <c r="AN27" s="29"/>
+      <c r="AO27" s="29"/>
+      <c r="AP27" s="29"/>
+      <c r="AQ27" s="29"/>
+      <c r="AR27" s="29"/>
+      <c r="AS27" s="29"/>
+      <c r="AT27" s="29"/>
+      <c r="AU27" s="29"/>
+      <c r="AV27" s="29"/>
+      <c r="AW27" s="29"/>
+      <c r="AX27" s="29"/>
+      <c r="AY27" s="29"/>
+      <c r="AZ27" s="29"/>
+      <c r="BA27" s="29"/>
+      <c r="BB27" s="29"/>
+      <c r="BC27" s="29"/>
+      <c r="BD27" s="29"/>
+      <c r="BE27" s="29"/>
+      <c r="BF27" s="29"/>
+      <c r="BG27" s="29"/>
+      <c r="BH27" s="29"/>
+      <c r="BI27" s="29"/>
+      <c r="BJ27" s="29"/>
+      <c r="BK27" s="29"/>
+      <c r="BL27" s="29"/>
+      <c r="BM27" s="29"/>
+      <c r="BN27" s="29"/>
+      <c r="BO27" s="29"/>
+      <c r="BP27" s="29"/>
+      <c r="BQ27" s="29"/>
+      <c r="BR27" s="29"/>
+      <c r="BS27" s="29"/>
+      <c r="BT27" s="29"/>
+      <c r="BU27" s="29"/>
+      <c r="BV27" s="29"/>
+      <c r="BW27" s="29"/>
+      <c r="BX27" s="29"/>
+      <c r="BY27" s="29"/>
+      <c r="BZ27" s="29"/>
+      <c r="CA27" s="29"/>
+      <c r="CB27" s="29"/>
+      <c r="CC27" s="29"/>
+      <c r="CD27" s="29"/>
+      <c r="CE27" s="29"/>
+      <c r="CF27" s="29"/>
+      <c r="CG27" s="29"/>
+      <c r="CH27" s="29"/>
+      <c r="CI27" s="29"/>
+      <c r="CJ27" s="29"/>
+      <c r="CK27" s="29"/>
+      <c r="CL27" s="29"/>
+      <c r="CM27" s="29"/>
+      <c r="CN27" s="29"/>
+      <c r="CO27" s="29"/>
+      <c r="CP27" s="29"/>
+      <c r="CQ27" s="29"/>
+      <c r="CR27" s="29"/>
+      <c r="CS27" s="29"/>
+      <c r="CT27" s="29"/>
+      <c r="CU27" s="29"/>
+      <c r="CV27"/>
+      <c r="CW27"/>
+      <c r="CX27"/>
+      <c r="CY27"/>
+      <c r="CZ27"/>
+      <c r="DA27"/>
+      <c r="DB27"/>
+      <c r="DC27"/>
+      <c r="DD27"/>
+      <c r="DE27"/>
+      <c r="DF27"/>
+      <c r="DG27"/>
+      <c r="DH27"/>
+      <c r="DI27"/>
+      <c r="DJ27"/>
+      <c r="DK27"/>
+      <c r="DL27"/>
+      <c r="DM27"/>
+      <c r="DN27"/>
+      <c r="DO27"/>
+      <c r="DP27"/>
     </row>
     <row r="28" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="42"/>
+      <c r="A28" s="42" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="29" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="42"/>
@@ -5360,46 +5317,52 @@
       <c r="A31" s="42"/>
     </row>
     <row r="32" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="42" t="s">
-        <v>26</v>
-      </c>
+      <c r="A32" s="42"/>
     </row>
     <row r="33" spans="1:7" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="42"/>
+    </row>
+    <row r="34" spans="1:7" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="43" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="14"/>
-      <c r="F35" s="44"/>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="15"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="14"/>
+      <c r="F37" s="44"/>
+    </row>
+    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D19 D24:D25">
-    <cfRule type="dataBar" priority="44">
+  <conditionalFormatting sqref="D7:D18 D26:D27 D21">
+    <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5412,21 +5375,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL25">
-    <cfRule type="expression" dxfId="50" priority="63">
+  <conditionalFormatting sqref="I5:BL27">
+    <cfRule type="expression" dxfId="20" priority="65">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL25">
-    <cfRule type="expression" dxfId="49" priority="57">
+  <conditionalFormatting sqref="I7:BL27">
+    <cfRule type="expression" dxfId="19" priority="59">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="60" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="dataBar" priority="30">
+  <conditionalFormatting sqref="D22">
+    <cfRule type="dataBar" priority="32">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5439,8 +5402,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D22">
-    <cfRule type="dataBar" priority="29">
+  <conditionalFormatting sqref="D23:D24">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5453,8 +5416,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
-    <cfRule type="dataBar" priority="28">
+  <conditionalFormatting sqref="D25">
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5467,69 +5430,97 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM5:BS25">
-    <cfRule type="expression" dxfId="23" priority="24">
+  <conditionalFormatting sqref="BM5:BS27">
+    <cfRule type="expression" dxfId="17" priority="26">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM7:BS25">
-    <cfRule type="expression" dxfId="22" priority="22">
+  <conditionalFormatting sqref="BM7:BS27">
+    <cfRule type="expression" dxfId="16" priority="24">
       <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="25" stopIfTrue="1">
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT5:BZ25">
-    <cfRule type="expression" dxfId="20" priority="21">
+  <conditionalFormatting sqref="BT5:BZ27">
+    <cfRule type="expression" dxfId="14" priority="23">
       <formula>AND(TODAY()&gt;=BT$5,TODAY()&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT7:BZ25">
-    <cfRule type="expression" dxfId="19" priority="19">
+  <conditionalFormatting sqref="BT7:BZ27">
+    <cfRule type="expression" dxfId="13" priority="21">
       <formula>AND(task_start&lt;=BT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BT$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="22" stopIfTrue="1">
       <formula>AND(task_end&gt;=BT$5,task_start&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA5:CG25">
-    <cfRule type="expression" dxfId="17" priority="18">
+  <conditionalFormatting sqref="CA5:CG27">
+    <cfRule type="expression" dxfId="11" priority="20">
       <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA7:CG25">
-    <cfRule type="expression" dxfId="16" priority="16">
+  <conditionalFormatting sqref="CA7:CG27">
+    <cfRule type="expression" dxfId="10" priority="18">
       <formula>AND(task_start&lt;=CA$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CA$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="19" stopIfTrue="1">
       <formula>AND(task_end&gt;=CA$5,task_start&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH5:CN25">
-    <cfRule type="expression" dxfId="14" priority="15">
+  <conditionalFormatting sqref="CH5:CN27">
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>AND(TODAY()&gt;=CH$5,TODAY()&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CH7:CN25">
-    <cfRule type="expression" dxfId="13" priority="13">
+  <conditionalFormatting sqref="CH7:CN27">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>AND(task_start&lt;=CH$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CH$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="16" stopIfTrue="1">
       <formula>AND(task_end&gt;=CH$5,task_start&lt;CI$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO5:CU25">
-    <cfRule type="expression" dxfId="11" priority="12">
+  <conditionalFormatting sqref="CO5:CU27">
+    <cfRule type="expression" dxfId="5" priority="14">
       <formula>AND(TODAY()&gt;=CO$5,TODAY()&lt;CP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CO7:CU25">
-    <cfRule type="expression" dxfId="10" priority="10">
+  <conditionalFormatting sqref="CO7:CU27">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>AND(task_start&lt;=CO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CO$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="13" stopIfTrue="1">
       <formula>AND(task_end&gt;=CO$5,task_start&lt;CP$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6AE55CE7-6CB7-404F-8607-7978CA94F771}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E9520B7C-A893-4A27-9CA2-64AC3FFA688F}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5559,7 +5550,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D19 D24:D25</xm:sqref>
+          <xm:sqref>D7:D18 D26:D27 D21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2BEE3156-7006-46B5-B47A-DD654311D6E0}">
@@ -5574,7 +5565,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D20</xm:sqref>
+          <xm:sqref>D22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{17C277CB-8C1C-42FE-8D62-1652FC5FBD84}">
@@ -5589,7 +5580,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D21:D22</xm:sqref>
+          <xm:sqref>D23:D24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2EED09A3-57CD-4D24-8416-966644C113F2}">
@@ -5604,7 +5595,37 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D23</xm:sqref>
+          <xm:sqref>D25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6AE55CE7-6CB7-404F-8607-7978CA94F771}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E9520B7C-A893-4A27-9CA2-64AC3FFA688F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D20</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5616,7 +5637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>